<commit_message>
Case Validation and sink_CEMI
</commit_message>
<xml_diff>
--- a/Data/CEMI_chapas.xlsx
+++ b/Data/CEMI_chapas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpern\Documents\GitHub\PyFlow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B0B1A3-07EF-4BBD-AB80-F5807C15D242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD1F553-8347-46CF-B67B-1B0A651126A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MBOM" sheetId="2" r:id="rId1"/>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7692789-1C38-476F-B78A-11B6D05AE770}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B3" t="s">
         <v>106</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B4" t="s">
         <v>107</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B5" t="s">
         <v>108</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B6" t="s">
         <v>109</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B7" t="s">
         <v>110</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B8" t="s">
         <v>111</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B9" t="s">
         <v>112</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B10" t="s">
         <v>113</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B11" t="s">
         <v>114</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B12" t="s">
         <v>115</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B13" t="s">
         <v>116</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B14" t="s">
         <v>117</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B15" t="s">
         <v>118</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B16" t="s">
         <v>119</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B17" t="s">
         <v>120</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B18" t="s">
         <v>121</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B19" t="s">
         <v>122</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B20" t="s">
         <v>123</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B21" t="s">
         <v>124</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B22" t="s">
         <v>125</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B23" t="s">
         <v>126</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B24" t="s">
         <v>127</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B25" t="s">
         <v>128</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B26" t="s">
         <v>129</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B27" t="s">
         <v>130</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B28" t="s">
         <v>131</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B29" t="s">
         <v>132</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B30" t="s">
         <v>133</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B31" t="s">
         <v>134</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B32" t="s">
         <v>135</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B33" t="s">
         <v>136</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B34" t="s">
         <v>137</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B35" t="s">
         <v>138</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B36" t="s">
         <v>139</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B37" t="s">
         <v>140</v>
@@ -2081,7 +2081,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B38" t="s">
         <v>141</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B39" t="s">
         <v>142</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B40" t="s">
         <v>143</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B41" t="s">
         <v>144</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B42" t="s">
         <v>145</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B43" t="s">
         <v>146</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B44" t="s">
         <v>147</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B45" t="s">
         <v>148</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B46" t="s">
         <v>149</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B47" t="s">
         <v>150</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B48" t="s">
         <v>151</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B49" t="s">
         <v>152</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B50" t="s">
         <v>153</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B51" t="s">
         <v>154</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B52" t="s">
         <v>155</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B53" t="s">
         <v>156</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B54" t="s">
         <v>157</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B55" t="s">
         <v>158</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B56" t="s">
         <v>159</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B57" t="s">
         <v>160</v>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B59" t="s">
         <v>162</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B60" t="s">
         <v>163</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B61" t="s">
         <v>164</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B62" t="s">
         <v>165</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B63" t="s">
         <v>166</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B64" t="s">
         <v>167</v>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B65" t="s">
         <v>168</v>
@@ -2893,7 +2893,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B66" t="s">
         <v>169</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B67" t="s">
         <v>170</v>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B68" t="s">
         <v>171</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B69" t="s">
         <v>172</v>
@@ -3009,7 +3009,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B70" t="s">
         <v>173</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B71" t="s">
         <v>174</v>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B72" t="s">
         <v>175</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B73" t="s">
         <v>176</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B74" t="s">
         <v>177</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B75" t="s">
         <v>178</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B76" t="s">
         <v>179</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B77" t="s">
         <v>180</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B78" t="s">
         <v>181</v>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B79" t="s">
         <v>182</v>
@@ -3299,7 +3299,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B80" t="s">
         <v>183</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B81" t="s">
         <v>184</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B82" t="s">
         <v>185</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B83" t="s">
         <v>186</v>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B84" t="s">
         <v>187</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B85" t="s">
         <v>188</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B86" t="s">
         <v>189</v>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B87" t="s">
         <v>190</v>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B88" t="s">
         <v>191</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B89" t="s">
         <v>192</v>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B90" t="s">
         <v>193</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>0</v>
+        <v>78.612300000000005</v>
       </c>
       <c r="B91" t="s">
         <v>194</v>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B33" ca="1" si="0">RAND()</f>
-        <v>0.12049778646906795</v>
+        <v>0.70823352183354038</v>
       </c>
       <c r="E2" t="s">
         <v>205</v>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0832116361762325E-2</v>
+        <v>0.13179784902751146</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53583920819100372</v>
+        <v>0.12245099614513888</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87064214551218422</v>
+        <v>0.65874118915785596</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -3814,7 +3814,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32339804803507688</v>
+        <v>0.26604149374730468</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11195060717059513</v>
+        <v>0.88816307916671655</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85859526917236662</v>
+        <v>0.10767286555106603</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84572574724215421</v>
+        <v>0.39060405606737814</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -3962,7 +3962,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66923192491931183</v>
+        <v>5.8479079477769869E-2</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18000115644839043</v>
+        <v>0.2239678162744726</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3938733939439294</v>
+        <v>0.93073981584365972</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -4073,7 +4073,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38684851479431226</v>
+        <v>0.9605369520853585</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34228868462118189</v>
+        <v>0.44940826752867624</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52679288664401935</v>
+        <v>0.4697709487525793</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53665158053090301</v>
+        <v>0.81977564546208415</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33228141348365603</v>
+        <v>0.71385395513140448</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25051132116471853</v>
+        <v>0.72355138963746546</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5509257173165776E-2</v>
+        <v>0.29959237212957568</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4609338100097442</v>
+        <v>0.46546037830777465</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83576005364923756</v>
+        <v>0.95959396255641061</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37434430263813501</v>
+        <v>0.41605020474058296</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -4443,7 +4443,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58893619360636273</v>
+        <v>0.62065817679922175</v>
       </c>
       <c r="E23">
         <v>21</v>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67959844390884117</v>
+        <v>0.18221950865022818</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72000754956787172</v>
+        <v>0.77538917863564427</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -4554,7 +4554,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78623574040952438</v>
+        <v>5.7821953097666468E-3</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62608167375364798</v>
+        <v>0.78427745629450707</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81250864521002242</v>
+        <v>0.10236067230001344</v>
       </c>
       <c r="E28">
         <v>26</v>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87855002799238069</v>
+        <v>0.78359138309340404</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67817495748734258</v>
+        <v>0.5080368510419967</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -4739,7 +4739,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42370636231069914</v>
+        <v>0.41570057052739073</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -4776,7 +4776,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44089186956593562</v>
+        <v>0.71481708779543485</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76919109234080008</v>
+        <v>0.10241069996784857</v>
       </c>
       <c r="E33">
         <v>31</v>
@@ -4850,7 +4850,7 @@
       </c>
       <c r="B34">
         <f t="shared" ref="B34:B65" ca="1" si="1">RAND()</f>
-        <v>0.71222713590674736</v>
+        <v>0.83328796601364707</v>
       </c>
       <c r="E34">
         <v>32</v>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61930846201475542</v>
+        <v>0.38849225477781801</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -4924,7 +4924,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1978004627334482</v>
+        <v>0.3523684613327952</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42909443632332478</v>
+        <v>0.28399080824444989</v>
       </c>
       <c r="E37">
         <v>35</v>
@@ -4998,7 +4998,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0560448814443473E-2</v>
+        <v>0.8564827514332376</v>
       </c>
       <c r="E38">
         <v>36</v>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46709368076632107</v>
+        <v>0.96195768445998076</v>
       </c>
       <c r="E39">
         <v>37</v>
@@ -5072,7 +5072,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3339195050363886E-2</v>
+        <v>0.96160941685279511</v>
       </c>
       <c r="E40">
         <v>38</v>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42890289711172358</v>
+        <v>0.32405678654183956</v>
       </c>
       <c r="E41">
         <v>39</v>
@@ -5146,7 +5146,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6220999037747138</v>
+        <v>0.74598055732657442</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -5183,7 +5183,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49459430780843261</v>
+        <v>0.77588465369314197</v>
       </c>
       <c r="E43">
         <v>41</v>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51642934912490324</v>
+        <v>0.11231536244808393</v>
       </c>
       <c r="E44">
         <v>42</v>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54215173388826254</v>
+        <v>5.7362995232448033E-2</v>
       </c>
       <c r="E45">
         <v>43</v>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68004949503426071</v>
+        <v>0.22843598399415399</v>
       </c>
       <c r="E46">
         <v>44</v>
@@ -5331,7 +5331,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80316196642620885</v>
+        <v>4.5294543271511722E-2</v>
       </c>
       <c r="E47">
         <v>45</v>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36822429248560906</v>
+        <v>0.25733400649598881</v>
       </c>
       <c r="E48">
         <v>46</v>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9811227102255532</v>
+        <v>0.6797784829078527</v>
       </c>
       <c r="E49">
         <v>47</v>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68295305222864644</v>
+        <v>0.10202937731879502</v>
       </c>
       <c r="E50">
         <v>48</v>
@@ -5479,7 +5479,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20012104523462149</v>
+        <v>0.47477253443051748</v>
       </c>
       <c r="E51">
         <v>49</v>
@@ -5516,7 +5516,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90134532494861541</v>
+        <v>3.5053987331373992E-2</v>
       </c>
       <c r="E52">
         <v>50</v>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39976857210612526</v>
+        <v>0.50210328018597394</v>
       </c>
       <c r="E53">
         <v>51</v>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22132748476528541</v>
+        <v>0.69616084580208948</v>
       </c>
       <c r="E54">
         <v>52</v>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22112950709990653</v>
+        <v>0.71837745407646547</v>
       </c>
       <c r="E55">
         <v>53</v>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93472783068958243</v>
+        <v>0.16960840187738624</v>
       </c>
       <c r="E56">
         <v>54</v>
@@ -5701,7 +5701,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78322124371582069</v>
+        <v>0.47003287206464262</v>
       </c>
       <c r="E57">
         <v>55</v>
@@ -5738,7 +5738,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6540190993026509</v>
+        <v>0.73449000675809684</v>
       </c>
       <c r="E58">
         <v>56</v>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93041436728083293</v>
+        <v>0.86790725619500531</v>
       </c>
       <c r="E59">
         <v>57</v>
@@ -5812,7 +5812,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69624377490240863</v>
+        <v>0.25653653710616686</v>
       </c>
       <c r="E60">
         <v>58</v>
@@ -5849,7 +5849,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81882715051443178</v>
+        <v>0.60475012211202794</v>
       </c>
       <c r="E61">
         <v>59</v>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55148417311654385</v>
+        <v>0.75851212266949219</v>
       </c>
       <c r="E62">
         <v>60</v>
@@ -5923,7 +5923,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97062742691172565</v>
+        <v>0.99191824823703956</v>
       </c>
       <c r="E63">
         <v>61</v>
@@ -5960,7 +5960,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80058774241188213</v>
+        <v>0.69819424624009929</v>
       </c>
       <c r="E64">
         <v>62</v>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79031768869792807</v>
+        <v>0.77404934435847184</v>
       </c>
       <c r="E65">
         <v>63</v>
@@ -6034,7 +6034,7 @@
       </c>
       <c r="B66">
         <f t="shared" ref="B66:B91" ca="1" si="2">RAND()</f>
-        <v>0.618206434245828</v>
+        <v>0.45645328163248222</v>
       </c>
       <c r="E66">
         <v>64</v>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12889693440229055</v>
+        <v>0.78319212261247562</v>
       </c>
       <c r="E67">
         <v>65</v>
@@ -6108,7 +6108,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26252427512914533</v>
+        <v>0.50384599908922567</v>
       </c>
       <c r="E68">
         <v>66</v>
@@ -6145,7 +6145,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="2"/>
-        <v>7.8246868001369263E-2</v>
+        <v>0.55405582350713267</v>
       </c>
       <c r="E69">
         <v>67</v>
@@ -6182,7 +6182,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="2"/>
-        <v>0.51406872527242131</v>
+        <v>9.919346792301631E-2</v>
       </c>
       <c r="E70">
         <v>68</v>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="2"/>
-        <v>0.99354662579591246</v>
+        <v>0.37257251402850911</v>
       </c>
       <c r="E71">
         <v>69</v>
@@ -6256,7 +6256,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44478347277046126</v>
+        <v>0.55139041479720974</v>
       </c>
       <c r="E72">
         <v>70</v>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10902822132246071</v>
+        <v>0.48601855971498231</v>
       </c>
       <c r="E73">
         <v>71</v>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="2"/>
-        <v>0.14819559170414964</v>
+        <v>0.19208238524659471</v>
       </c>
       <c r="E74">
         <v>72</v>
@@ -6367,7 +6367,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="2"/>
-        <v>0.20013557602216958</v>
+        <v>0.34580453941559997</v>
       </c>
       <c r="E75">
         <v>73</v>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="2"/>
-        <v>0.62998633113649394</v>
+        <v>0.99660286636085726</v>
       </c>
       <c r="E76">
         <v>74</v>
@@ -6441,7 +6441,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="2"/>
-        <v>0.96168022774643958</v>
+        <v>0.66459833523693179</v>
       </c>
       <c r="E77">
         <v>75</v>
@@ -6478,7 +6478,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="2"/>
-        <v>0.13228734745186188</v>
+        <v>0.57379366973928247</v>
       </c>
       <c r="E78">
         <v>76</v>
@@ -6515,7 +6515,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="2"/>
-        <v>0.42929954806433501</v>
+        <v>0.39514027071341928</v>
       </c>
       <c r="E79">
         <v>77</v>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19628256197656213</v>
+        <v>0.44688206308191769</v>
       </c>
       <c r="E80">
         <v>78</v>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="2"/>
-        <v>0.4680708099748625</v>
+        <v>0.7781543331134726</v>
       </c>
       <c r="E81">
         <v>79</v>
@@ -6626,7 +6626,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="2"/>
-        <v>7.4269335444437923E-2</v>
+        <v>0.2141569330013452</v>
       </c>
       <c r="E82">
         <v>80</v>
@@ -6663,7 +6663,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="2"/>
-        <v>0.72659506623625303</v>
+        <v>0.78093423805303197</v>
       </c>
       <c r="E83">
         <v>81</v>
@@ -6700,7 +6700,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9067778237634392E-2</v>
+        <v>0.93906738883425223</v>
       </c>
       <c r="E84">
         <v>82</v>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89557956312707021</v>
+        <v>0.88282056702147282</v>
       </c>
       <c r="E85">
         <v>83</v>
@@ -6774,7 +6774,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19548840336036166</v>
+        <v>0.55381709257446243</v>
       </c>
       <c r="E86">
         <v>84</v>
@@ -6811,7 +6811,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="2"/>
-        <v>0.96712887183913532</v>
+        <v>0.61835859026211426</v>
       </c>
       <c r="E87">
         <v>85</v>
@@ -6848,7 +6848,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="2"/>
-        <v>0.40418889188686891</v>
+        <v>0.92292831173603229</v>
       </c>
       <c r="E88">
         <v>86</v>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="2"/>
-        <v>0.62669549975664418</v>
+        <v>0.79506146119968335</v>
       </c>
       <c r="E89">
         <v>87</v>
@@ -6922,7 +6922,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="2"/>
-        <v>0.95296833075452902</v>
+        <v>0.88516775481007348</v>
       </c>
       <c r="E90">
         <v>88</v>
@@ -6959,7 +6959,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="2"/>
-        <v>0.57499076401468241</v>
+        <v>0.42837951913475358</v>
       </c>
       <c r="E91">
         <v>89</v>

</xml_diff>